<commit_message>
Created list of herbarium samples
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C534AD70-0C8E-4ECC-9D6F-97FF05D5D719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C91FA-D4BB-417B-AE12-F7667BF2E46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A9E7AED2-81D5-42E0-9111-304D65E4884B}"/>
   </bookViews>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B8EB86-14DD-425D-A2EB-E983309B0F93}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated scutellaria list to include seed availability
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C91FA-D4BB-417B-AE12-F7667BF2E46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCB69E1-BECC-4CE4-9664-0827E3C9672D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A9E7AED2-81D5-42E0-9111-304D65E4884B}"/>
+    <workbookView xWindow="14745" yWindow="6420" windowWidth="15375" windowHeight="8325" xr2:uid="{A9E7AED2-81D5-42E0-9111-304D65E4884B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>shoots</t>
   </si>
   <si>
-    <t>laterifolia</t>
-  </si>
-  <si>
     <t>sapphirina</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>17-1</t>
+  </si>
+  <si>
+    <t>lateriflora</t>
   </si>
 </sst>
 </file>
@@ -704,7 +704,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -746,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -774,10 +774,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -788,10 +788,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -802,10 +802,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -813,13 +813,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -827,13 +827,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -841,13 +841,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -855,13 +855,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -869,13 +869,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -883,13 +883,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -897,13 +897,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -911,13 +911,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
         <v>21</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -925,13 +925,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -939,13 +939,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -967,13 +967,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -981,13 +981,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -995,13 +995,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1009,13 +1009,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1065,13 +1065,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -1079,13 +1079,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
         <v>39</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -1093,13 +1093,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -1121,13 +1121,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1135,13 +1135,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
         <v>44</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -1149,13 +1149,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
         <v>46</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>47</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -1163,13 +1163,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>48</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -1177,13 +1177,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
         <v>50</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -1191,13 +1191,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
         <v>52</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -1205,13 +1205,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -1219,13 +1219,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
         <v>55</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
-        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -1233,27 +1233,27 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>58</v>
-      </c>
-      <c r="D38" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1275,13 +1275,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" t="s">
         <v>62</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" t="s">
-        <v>63</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -1289,13 +1289,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
         <v>64</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" t="s">
-        <v>65</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
@@ -1303,13 +1303,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -1317,27 +1317,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>68</v>
-      </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" t="s">
         <v>69</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" t="s">
-        <v>70</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updated herbarium list with correct numbering
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -1,37 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCB69E1-BECC-4CE4-9664-0827E3C9672D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E735DF7C-F744-4E22-8581-23572B4593D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14745" yWindow="6420" windowWidth="15375" windowHeight="8325" xr2:uid="{A9E7AED2-81D5-42E0-9111-304D65E4884B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="206">
   <si>
     <t>Label</t>
   </si>
@@ -335,13 +343,344 @@
   </si>
   <si>
     <t>lateriflora</t>
+  </si>
+  <si>
+    <t>NYBG03</t>
+  </si>
+  <si>
+    <t>S. angustifolia ssp. micranthum</t>
+  </si>
+  <si>
+    <t>NYBG04</t>
+  </si>
+  <si>
+    <t>S. angustifolia ssp. angustifolia</t>
+  </si>
+  <si>
+    <t>NYBG05</t>
+  </si>
+  <si>
+    <t>S. antirrhinoides</t>
+  </si>
+  <si>
+    <t>NYBG07</t>
+  </si>
+  <si>
+    <t>S. brittonii</t>
+  </si>
+  <si>
+    <t>NYBG08</t>
+  </si>
+  <si>
+    <t>S. californica</t>
+  </si>
+  <si>
+    <t>NYBG09</t>
+  </si>
+  <si>
+    <t>S. coccinea</t>
+  </si>
+  <si>
+    <t>NYBG10</t>
+  </si>
+  <si>
+    <t>S. drumondii</t>
+  </si>
+  <si>
+    <t>NYBG13</t>
+  </si>
+  <si>
+    <t>S. glabriuscula</t>
+  </si>
+  <si>
+    <t>NYBG14</t>
+  </si>
+  <si>
+    <t>S. havanensis</t>
+  </si>
+  <si>
+    <t>NYBG15</t>
+  </si>
+  <si>
+    <t>S. holmgrenierum</t>
+  </si>
+  <si>
+    <t>NYBG17</t>
+  </si>
+  <si>
+    <t>S. incana</t>
+  </si>
+  <si>
+    <t>NYBG19</t>
+  </si>
+  <si>
+    <t>S. leonardii</t>
+  </si>
+  <si>
+    <t>NYBG22</t>
+  </si>
+  <si>
+    <t>S. multiglandulosa</t>
+  </si>
+  <si>
+    <t>NYBG23</t>
+  </si>
+  <si>
+    <t>NYBG25</t>
+  </si>
+  <si>
+    <t>S. sapphirina</t>
+  </si>
+  <si>
+    <t>NYBG29</t>
+  </si>
+  <si>
+    <t>NYBG30</t>
+  </si>
+  <si>
+    <t>S. racemosa</t>
+  </si>
+  <si>
+    <t>NYBG32</t>
+  </si>
+  <si>
+    <t>NYBG38</t>
+  </si>
+  <si>
+    <t>S. blepharophylla</t>
+  </si>
+  <si>
+    <t>NYBG42</t>
+  </si>
+  <si>
+    <t>S. hispidula</t>
+  </si>
+  <si>
+    <t>NYBG44</t>
+  </si>
+  <si>
+    <t>S. guatemalensis</t>
+  </si>
+  <si>
+    <t>NYBG48</t>
+  </si>
+  <si>
+    <t>S. lutea</t>
+  </si>
+  <si>
+    <t>NYBG50</t>
+  </si>
+  <si>
+    <t>S. purpurascens</t>
+  </si>
+  <si>
+    <t>NYBG51</t>
+  </si>
+  <si>
+    <t>S. seleriana</t>
+  </si>
+  <si>
+    <t>S. suffrutscens</t>
+  </si>
+  <si>
+    <t>NYBG56</t>
+  </si>
+  <si>
+    <t>S. przewalskii</t>
+  </si>
+  <si>
+    <t>NYBG57</t>
+  </si>
+  <si>
+    <t>S. scordiifolia</t>
+  </si>
+  <si>
+    <t>NYBG58</t>
+  </si>
+  <si>
+    <t>S. discolor</t>
+  </si>
+  <si>
+    <t>NYBG60</t>
+  </si>
+  <si>
+    <t>S. multicularis</t>
+  </si>
+  <si>
+    <t>NYBG61</t>
+  </si>
+  <si>
+    <t>S. oblonga</t>
+  </si>
+  <si>
+    <t>NYBG62</t>
+  </si>
+  <si>
+    <t>S. heterophylla</t>
+  </si>
+  <si>
+    <t>NYBG63</t>
+  </si>
+  <si>
+    <t>S. heydei</t>
+  </si>
+  <si>
+    <t>NYBG64</t>
+  </si>
+  <si>
+    <t>S. javanica</t>
+  </si>
+  <si>
+    <t>NYBG65</t>
+  </si>
+  <si>
+    <t>S. pinnatifida</t>
+  </si>
+  <si>
+    <t>NYBG66</t>
+  </si>
+  <si>
+    <t>S. prostrata</t>
+  </si>
+  <si>
+    <t>NYBG67</t>
+  </si>
+  <si>
+    <t>S. peregrina</t>
+  </si>
+  <si>
+    <t>NYBG68</t>
+  </si>
+  <si>
+    <t>S. relenorskyi</t>
+  </si>
+  <si>
+    <t>NYBG69</t>
+  </si>
+  <si>
+    <t>S. angulosa</t>
+  </si>
+  <si>
+    <t>NYBG71</t>
+  </si>
+  <si>
+    <t>S. paucifolia</t>
+  </si>
+  <si>
+    <t>NYBG72</t>
+  </si>
+  <si>
+    <t>S. sumatrana</t>
+  </si>
+  <si>
+    <t>NYBG73</t>
+  </si>
+  <si>
+    <t>S. javalambrensis</t>
+  </si>
+  <si>
+    <t>NYBG74</t>
+  </si>
+  <si>
+    <t>S. leptosiplonsipkon</t>
+  </si>
+  <si>
+    <t>FLAS01</t>
+  </si>
+  <si>
+    <t>S. arenicola</t>
+  </si>
+  <si>
+    <t>FLAS02</t>
+  </si>
+  <si>
+    <t>FLAS04</t>
+  </si>
+  <si>
+    <t>S. elliptica</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLAS05</t>
+  </si>
+  <si>
+    <t>S. integrifolia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLAS06</t>
+  </si>
+  <si>
+    <t>S. multiglandulosa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLAS07</t>
+  </si>
+  <si>
+    <t>S. racemosa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S.hastifolia</t>
+  </si>
+  <si>
+    <t>S.arenicola</t>
+  </si>
+  <si>
+    <t>S.tournefortii</t>
+  </si>
+  <si>
+    <t>S.baicalensis</t>
+  </si>
+  <si>
+    <t>S.barbata</t>
+  </si>
+  <si>
+    <t>S.indica</t>
+  </si>
+  <si>
+    <t>S.Pekinesis</t>
+  </si>
+  <si>
+    <t>S.dependens</t>
+  </si>
+  <si>
+    <t>S.strigillosa</t>
+  </si>
+  <si>
+    <t>S.insignis</t>
+  </si>
+  <si>
+    <t>S. muriculata</t>
+  </si>
+  <si>
+    <t>S. pseudoserrata</t>
+  </si>
+  <si>
+    <t>Dry Weight</t>
+  </si>
+  <si>
+    <r>
+      <t>Solvent volume for 10000 ppm (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µL)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +695,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -700,20 +1046,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B8EB86-14DD-425D-A2EB-E983309B0F93}">
-  <dimension ref="A1:D50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -726,8 +1074,14 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -741,7 +1095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -755,7 +1109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -769,7 +1123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -783,7 +1137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -797,7 +1151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -811,7 +1165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -825,7 +1179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -839,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -853,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -867,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -881,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -895,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -909,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -923,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1161,7 +1515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
@@ -1175,7 +1529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
@@ -1189,7 +1543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>51</v>
       </c>
@@ -1203,7 +1557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1217,7 +1571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -1231,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -1245,7 +1599,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1259,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
@@ -1273,7 +1627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
@@ -1287,7 +1641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -1301,7 +1655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -1315,7 +1669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
@@ -1329,7 +1683,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -1343,20 +1697,793 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>31</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="F46">
+        <f>E46*1000/10*1000</f>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>32</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="F47">
+        <f t="shared" ref="F47:F75" si="0">E47*1000/10*1000</f>
+        <v>1529.9999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>33</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>909.99999999999989</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>34</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49">
+        <v>1.35E-2</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>35</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>470.00000000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>36</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>37</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>38</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>880.00000000000011</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>39</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>40</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55">
+        <v>1.29E-2</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>41</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>42</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E57">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>43</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>679.99999999999989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>44</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59">
+        <v>1.38E-2</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>45</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>46</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>570.00000000000011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>47</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E62">
+        <v>1.03E-2</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>48</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>49</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E64">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>50</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>51</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>1119.9999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>52</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E67">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>53</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68">
+        <v>1.38E-2</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="0"/>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>54</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E69">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="0"/>
+        <v>1640.0000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>55</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E70">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="0"/>
+        <v>1990.0000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>56</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>57</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72">
+        <v>2.87E-2</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="0"/>
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>58</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E73">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>59</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="0"/>
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>60</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E75">
+        <v>1.23E-2</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="0"/>
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>61</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>62</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>63</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>64</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>65</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>66</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>67</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>68</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>69</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>70</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>71</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>72</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>73</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>74</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>75</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>76</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>77</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>78</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="3" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added weights and calculated solvent volumes for herbarium samples 31-78
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E735DF7C-F744-4E22-8581-23572B4593D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC164690-D3C9-4FC0-8F56-95AA16343260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1729,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
       <c r="F47">
-        <f t="shared" ref="F47:F75" si="0">E47*1000/10*1000</f>
+        <f t="shared" ref="F47:F93" si="0">E47*1000/10*1000</f>
         <v>1529.9999999999998</v>
       </c>
     </row>
@@ -2247,6 +2247,13 @@
       <c r="C76" s="3" t="s">
         <v>158</v>
       </c>
+      <c r="E76">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="0"/>
+        <v>7600</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -2258,6 +2265,13 @@
       <c r="C77" s="3" t="s">
         <v>160</v>
       </c>
+      <c r="E77">
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="0"/>
+        <v>5550</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -2269,6 +2283,13 @@
       <c r="C78" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="E78">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
@@ -2280,6 +2301,13 @@
       <c r="C79" s="3" t="s">
         <v>164</v>
       </c>
+      <c r="E79">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="0"/>
+        <v>2570</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -2291,8 +2319,15 @@
       <c r="C80" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>2.1899999999999999E-2</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="0"/>
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>66</v>
       </c>
@@ -2302,8 +2337,15 @@
       <c r="C81" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="0"/>
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>67</v>
       </c>
@@ -2313,8 +2355,15 @@
       <c r="C82" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="0"/>
+        <v>2219.9999999999995</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>68</v>
       </c>
@@ -2324,8 +2373,15 @@
       <c r="C83" s="3" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="0"/>
+        <v>880.00000000000011</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>69</v>
       </c>
@@ -2335,8 +2391,15 @@
       <c r="C84" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>0.19719999999999999</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="0"/>
+        <v>19720</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>70</v>
       </c>
@@ -2346,8 +2409,15 @@
       <c r="C85" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="0"/>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>71</v>
       </c>
@@ -2357,8 +2427,15 @@
       <c r="C86" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="0"/>
+        <v>3230.0000000000005</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>72</v>
       </c>
@@ -2368,8 +2445,15 @@
       <c r="C87" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>73</v>
       </c>
@@ -2379,8 +2463,15 @@
       <c r="C88" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="0"/>
+        <v>840.00000000000011</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>74</v>
       </c>
@@ -2390,8 +2481,15 @@
       <c r="C89" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="0"/>
+        <v>1640.0000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>75</v>
       </c>
@@ -2401,8 +2499,15 @@
       <c r="C90" s="3" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>76</v>
       </c>
@@ -2412,8 +2517,15 @@
       <c r="C91" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="0"/>
+        <v>459.99999999999994</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>77</v>
       </c>
@@ -2423,8 +2535,15 @@
       <c r="C92" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="0"/>
+        <v>1569.9999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>78</v>
       </c>
@@ -2434,18 +2553,25 @@
       <c r="C93" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>3.39E-2</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="0"/>
+        <v>3389.9999999999995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C94" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C95" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C96" s="3" t="s">
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
Created scripts for generating alignment and variant calling statistics
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC164690-D3C9-4FC0-8F56-95AA16343260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A6D66D-F69F-477A-924F-24F589B76F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21045" yWindow="12180" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="196">
   <si>
     <t>Label</t>
   </si>
@@ -620,36 +620,6 @@
   <si>
     <t>S. racemosa</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S.hastifolia</t>
-  </si>
-  <si>
-    <t>S.arenicola</t>
-  </si>
-  <si>
-    <t>S.tournefortii</t>
-  </si>
-  <si>
-    <t>S.baicalensis</t>
-  </si>
-  <si>
-    <t>S.barbata</t>
-  </si>
-  <si>
-    <t>S.indica</t>
-  </si>
-  <si>
-    <t>S.Pekinesis</t>
-  </si>
-  <si>
-    <t>S.dependens</t>
-  </si>
-  <si>
-    <t>S.strigillosa</t>
-  </si>
-  <si>
-    <t>S.insignis</t>
   </si>
   <si>
     <t>S. muriculata</t>
@@ -1047,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,10 +1045,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1939,7 +1909,7 @@
         <v>127</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E59">
         <v>1.38E-2</v>
@@ -1975,7 +1945,7 @@
         <v>130</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E61">
         <v>5.7000000000000002E-3</v>
@@ -2559,56 +2529,6 @@
       <c r="F93">
         <f t="shared" si="0"/>
         <v>3389.9999999999995</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C94" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C95" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C96" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C103" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started regenerating PCA plot with new herbarium samples
</commit_message>
<xml_diff>
--- a/data/herbariumList.xlsx
+++ b/data/herbariumList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A6D66D-F69F-477A-924F-24F589B76F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306E534-9146-45CD-A18A-21DA172AEC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="12180" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="193">
   <si>
     <t>Label</t>
   </si>
@@ -348,284 +348,142 @@
     <t>NYBG03</t>
   </si>
   <si>
-    <t>S. angustifolia ssp. micranthum</t>
-  </si>
-  <si>
     <t>NYBG04</t>
   </si>
   <si>
-    <t>S. angustifolia ssp. angustifolia</t>
-  </si>
-  <si>
     <t>NYBG05</t>
   </si>
   <si>
-    <t>S. antirrhinoides</t>
-  </si>
-  <si>
     <t>NYBG07</t>
   </si>
   <si>
-    <t>S. brittonii</t>
-  </si>
-  <si>
     <t>NYBG08</t>
   </si>
   <si>
-    <t>S. californica</t>
-  </si>
-  <si>
     <t>NYBG09</t>
   </si>
   <si>
-    <t>S. coccinea</t>
-  </si>
-  <si>
     <t>NYBG10</t>
   </si>
   <si>
-    <t>S. drumondii</t>
-  </si>
-  <si>
     <t>NYBG13</t>
   </si>
   <si>
-    <t>S. glabriuscula</t>
-  </si>
-  <si>
     <t>NYBG14</t>
   </si>
   <si>
-    <t>S. havanensis</t>
-  </si>
-  <si>
     <t>NYBG15</t>
   </si>
   <si>
-    <t>S. holmgrenierum</t>
-  </si>
-  <si>
     <t>NYBG17</t>
   </si>
   <si>
-    <t>S. incana</t>
-  </si>
-  <si>
     <t>NYBG19</t>
   </si>
   <si>
-    <t>S. leonardii</t>
-  </si>
-  <si>
     <t>NYBG22</t>
   </si>
   <si>
-    <t>S. multiglandulosa</t>
-  </si>
-  <si>
     <t>NYBG23</t>
   </si>
   <si>
     <t>NYBG25</t>
   </si>
   <si>
-    <t>S. sapphirina</t>
-  </si>
-  <si>
     <t>NYBG29</t>
   </si>
   <si>
     <t>NYBG30</t>
   </si>
   <si>
-    <t>S. racemosa</t>
-  </si>
-  <si>
     <t>NYBG32</t>
   </si>
   <si>
     <t>NYBG38</t>
   </si>
   <si>
-    <t>S. blepharophylla</t>
-  </si>
-  <si>
     <t>NYBG42</t>
   </si>
   <si>
-    <t>S. hispidula</t>
-  </si>
-  <si>
     <t>NYBG44</t>
   </si>
   <si>
-    <t>S. guatemalensis</t>
-  </si>
-  <si>
     <t>NYBG48</t>
   </si>
   <si>
-    <t>S. lutea</t>
-  </si>
-  <si>
     <t>NYBG50</t>
   </si>
   <si>
-    <t>S. purpurascens</t>
-  </si>
-  <si>
     <t>NYBG51</t>
   </si>
   <si>
-    <t>S. seleriana</t>
-  </si>
-  <si>
-    <t>S. suffrutscens</t>
-  </si>
-  <si>
     <t>NYBG56</t>
   </si>
   <si>
-    <t>S. przewalskii</t>
-  </si>
-  <si>
     <t>NYBG57</t>
   </si>
   <si>
-    <t>S. scordiifolia</t>
-  </si>
-  <si>
     <t>NYBG58</t>
   </si>
   <si>
-    <t>S. discolor</t>
-  </si>
-  <si>
     <t>NYBG60</t>
   </si>
   <si>
-    <t>S. multicularis</t>
-  </si>
-  <si>
     <t>NYBG61</t>
   </si>
   <si>
-    <t>S. oblonga</t>
-  </si>
-  <si>
     <t>NYBG62</t>
   </si>
   <si>
-    <t>S. heterophylla</t>
-  </si>
-  <si>
     <t>NYBG63</t>
   </si>
   <si>
-    <t>S. heydei</t>
-  </si>
-  <si>
     <t>NYBG64</t>
   </si>
   <si>
-    <t>S. javanica</t>
-  </si>
-  <si>
     <t>NYBG65</t>
   </si>
   <si>
-    <t>S. pinnatifida</t>
-  </si>
-  <si>
     <t>NYBG66</t>
   </si>
   <si>
-    <t>S. prostrata</t>
-  </si>
-  <si>
     <t>NYBG67</t>
   </si>
   <si>
-    <t>S. peregrina</t>
-  </si>
-  <si>
     <t>NYBG68</t>
   </si>
   <si>
-    <t>S. relenorskyi</t>
-  </si>
-  <si>
     <t>NYBG69</t>
   </si>
   <si>
-    <t>S. angulosa</t>
-  </si>
-  <si>
     <t>NYBG71</t>
   </si>
   <si>
-    <t>S. paucifolia</t>
-  </si>
-  <si>
     <t>NYBG72</t>
   </si>
   <si>
-    <t>S. sumatrana</t>
-  </si>
-  <si>
     <t>NYBG73</t>
   </si>
   <si>
-    <t>S. javalambrensis</t>
-  </si>
-  <si>
     <t>NYBG74</t>
   </si>
   <si>
-    <t>S. leptosiplonsipkon</t>
-  </si>
-  <si>
     <t>FLAS01</t>
   </si>
   <si>
-    <t>S. arenicola</t>
-  </si>
-  <si>
     <t>FLAS02</t>
   </si>
   <si>
     <t>FLAS04</t>
   </si>
   <si>
-    <t>S. elliptica</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FLAS05</t>
   </si>
   <si>
-    <t>S. integrifolia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FLAS06</t>
   </si>
   <si>
-    <t>S. multiglandulosa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FLAS07</t>
-  </si>
-  <si>
-    <t>S. racemosa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S. muriculata</t>
-  </si>
-  <si>
-    <t>S. pseudoserrata</t>
   </si>
   <si>
     <t>Dry Weight</t>
@@ -644,6 +502,135 @@
       </rPr>
       <t>µL)</t>
     </r>
+  </si>
+  <si>
+    <t>angustifolia ssp. angustifolia</t>
+  </si>
+  <si>
+    <t>antirrhinoides</t>
+  </si>
+  <si>
+    <t>brittonii</t>
+  </si>
+  <si>
+    <t>californica</t>
+  </si>
+  <si>
+    <t>coccinea</t>
+  </si>
+  <si>
+    <t>drumondii</t>
+  </si>
+  <si>
+    <t>glabriuscula</t>
+  </si>
+  <si>
+    <t>havanensis</t>
+  </si>
+  <si>
+    <t>holmgrenierum</t>
+  </si>
+  <si>
+    <t>incana</t>
+  </si>
+  <si>
+    <t>leonardii</t>
+  </si>
+  <si>
+    <t>multiglandulosa</t>
+  </si>
+  <si>
+    <t>muriculata</t>
+  </si>
+  <si>
+    <t>pseudoserrata</t>
+  </si>
+  <si>
+    <t>racemosa</t>
+  </si>
+  <si>
+    <t>blepharophylla</t>
+  </si>
+  <si>
+    <t>hispidula</t>
+  </si>
+  <si>
+    <t>guatemalensis</t>
+  </si>
+  <si>
+    <t>lutea</t>
+  </si>
+  <si>
+    <t>purpurascens</t>
+  </si>
+  <si>
+    <t>seleriana</t>
+  </si>
+  <si>
+    <t>suffrutscens</t>
+  </si>
+  <si>
+    <t>przewalskii</t>
+  </si>
+  <si>
+    <t>scordiifolia</t>
+  </si>
+  <si>
+    <t>discolor</t>
+  </si>
+  <si>
+    <t>multicularis</t>
+  </si>
+  <si>
+    <t>oblonga</t>
+  </si>
+  <si>
+    <t>heterophylla</t>
+  </si>
+  <si>
+    <t>heydei</t>
+  </si>
+  <si>
+    <t>javanica</t>
+  </si>
+  <si>
+    <t>pinnatifida</t>
+  </si>
+  <si>
+    <t>prostrata</t>
+  </si>
+  <si>
+    <t>peregrina</t>
+  </si>
+  <si>
+    <t>relenorskyi</t>
+  </si>
+  <si>
+    <t>angulosa</t>
+  </si>
+  <si>
+    <t>paucifolia</t>
+  </si>
+  <si>
+    <t>sumatrana</t>
+  </si>
+  <si>
+    <t>javalambrensis</t>
+  </si>
+  <si>
+    <t>leptosiplonsipkon</t>
+  </si>
+  <si>
+    <t>arenicola</t>
+  </si>
+  <si>
+    <t>elliptica</t>
+  </si>
+  <si>
+    <t>integrifolia</t>
+  </si>
+  <si>
+    <t>angustifolia ssp. micranthum</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,10 +1032,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,7 +1662,10 @@
         <v>101</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>102</v>
+        <v>192</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
       </c>
       <c r="E46">
         <v>7.3000000000000001E-3</v>
@@ -1690,10 +1680,13 @@
         <v>32</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>104</v>
+        <v>150</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
       </c>
       <c r="E47">
         <v>1.5299999999999999E-2</v>
@@ -1708,10 +1701,13 @@
         <v>33</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>106</v>
+        <v>151</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
       </c>
       <c r="E48">
         <v>9.1000000000000004E-3</v>
@@ -1726,10 +1722,13 @@
         <v>34</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>108</v>
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
       </c>
       <c r="E49">
         <v>1.35E-2</v>
@@ -1744,10 +1743,13 @@
         <v>35</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>110</v>
+        <v>153</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
       </c>
       <c r="E50">
         <v>4.7000000000000002E-3</v>
@@ -1762,10 +1764,13 @@
         <v>36</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>112</v>
+        <v>154</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
       </c>
       <c r="E51">
         <v>5.1000000000000004E-3</v>
@@ -1780,10 +1785,13 @@
         <v>37</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>114</v>
+        <v>155</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
       </c>
       <c r="E52">
         <v>2.1000000000000001E-2</v>
@@ -1798,10 +1806,13 @@
         <v>38</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>116</v>
+        <v>156</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
       </c>
       <c r="E53">
         <v>8.8000000000000005E-3</v>
@@ -1816,10 +1827,13 @@
         <v>39</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>118</v>
+        <v>157</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
       </c>
       <c r="E54">
         <v>1.5900000000000001E-2</v>
@@ -1834,10 +1848,13 @@
         <v>40</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>120</v>
+        <v>158</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
       </c>
       <c r="E55">
         <v>1.29E-2</v>
@@ -1852,10 +1869,13 @@
         <v>41</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>122</v>
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
       </c>
       <c r="E56">
         <v>6.0000000000000001E-3</v>
@@ -1870,10 +1890,13 @@
         <v>42</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>124</v>
+        <v>160</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
       </c>
       <c r="E57">
         <v>8.9999999999999993E-3</v>
@@ -1888,10 +1911,13 @@
         <v>43</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>126</v>
+        <v>161</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
       </c>
       <c r="E58">
         <v>6.7999999999999996E-3</v>
@@ -1906,10 +1932,13 @@
         <v>44</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
       </c>
       <c r="E59">
         <v>1.38E-2</v>
@@ -1924,10 +1953,13 @@
         <v>45</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>129</v>
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
       </c>
       <c r="E60">
         <v>1.1900000000000001E-2</v>
@@ -1942,10 +1974,13 @@
         <v>46</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>193</v>
+        <v>163</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
       </c>
       <c r="E61">
         <v>5.7000000000000002E-3</v>
@@ -1960,10 +1995,13 @@
         <v>47</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>132</v>
+        <v>164</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
       </c>
       <c r="E62">
         <v>1.03E-2</v>
@@ -1978,10 +2016,13 @@
         <v>48</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>129</v>
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
       </c>
       <c r="E63">
         <v>2.0500000000000001E-2</v>
@@ -1996,10 +2037,13 @@
         <v>49</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>135</v>
+        <v>165</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
       </c>
       <c r="E64">
         <v>9.5999999999999992E-3</v>
@@ -2014,10 +2058,13 @@
         <v>50</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>137</v>
+        <v>166</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
       </c>
       <c r="E65">
         <v>6.1999999999999998E-3</v>
@@ -2032,10 +2079,13 @@
         <v>51</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>139</v>
+        <v>167</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
       </c>
       <c r="E66">
         <v>1.12E-2</v>
@@ -2050,10 +2100,13 @@
         <v>52</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>141</v>
+        <v>168</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
       </c>
       <c r="E67">
         <v>2.2499999999999999E-2</v>
@@ -2068,10 +2121,13 @@
         <v>53</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>143</v>
+        <v>169</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
       </c>
       <c r="E68">
         <v>1.38E-2</v>
@@ -2086,10 +2142,13 @@
         <v>54</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>145</v>
+        <v>170</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
       </c>
       <c r="E69">
         <v>1.6400000000000001E-2</v>
@@ -2107,7 +2166,10 @@
         <v>97</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>146</v>
+        <v>171</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
       </c>
       <c r="E70">
         <v>1.9900000000000001E-2</v>
@@ -2122,10 +2184,13 @@
         <v>56</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>148</v>
+        <v>172</v>
+      </c>
+      <c r="D71" t="s">
+        <v>7</v>
       </c>
       <c r="E71">
         <v>1.4E-2</v>
@@ -2140,10 +2205,13 @@
         <v>57</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>150</v>
+        <v>173</v>
+      </c>
+      <c r="D72" t="s">
+        <v>7</v>
       </c>
       <c r="E72">
         <v>2.87E-2</v>
@@ -2158,10 +2226,13 @@
         <v>58</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>152</v>
+        <v>174</v>
+      </c>
+      <c r="D73" t="s">
+        <v>4</v>
       </c>
       <c r="E73">
         <v>6.4000000000000003E-3</v>
@@ -2176,10 +2247,13 @@
         <v>59</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>154</v>
+        <v>175</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
       </c>
       <c r="E74">
         <v>8.2500000000000004E-2</v>
@@ -2194,10 +2268,13 @@
         <v>60</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>156</v>
+        <v>176</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
       </c>
       <c r="E75">
         <v>1.23E-2</v>
@@ -2212,10 +2289,13 @@
         <v>61</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>158</v>
+        <v>177</v>
+      </c>
+      <c r="D76" t="s">
+        <v>58</v>
       </c>
       <c r="E76">
         <v>7.5999999999999998E-2</v>
@@ -2230,10 +2310,13 @@
         <v>62</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>160</v>
+        <v>178</v>
+      </c>
+      <c r="D77" t="s">
+        <v>4</v>
       </c>
       <c r="E77">
         <v>5.5500000000000001E-2</v>
@@ -2248,10 +2331,13 @@
         <v>63</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>162</v>
+        <v>179</v>
+      </c>
+      <c r="D78" t="s">
+        <v>4</v>
       </c>
       <c r="E78">
         <v>2.9000000000000001E-2</v>
@@ -2266,10 +2352,13 @@
         <v>64</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>164</v>
+        <v>180</v>
+      </c>
+      <c r="D79" t="s">
+        <v>7</v>
       </c>
       <c r="E79">
         <v>2.5700000000000001E-2</v>
@@ -2284,10 +2373,13 @@
         <v>65</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>166</v>
+        <v>181</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
       </c>
       <c r="E80">
         <v>2.1899999999999999E-2</v>
@@ -2302,10 +2394,13 @@
         <v>66</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>168</v>
+        <v>182</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
       </c>
       <c r="E81">
         <v>1.0200000000000001E-2</v>
@@ -2320,10 +2415,13 @@
         <v>67</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>170</v>
+        <v>183</v>
+      </c>
+      <c r="D82" t="s">
+        <v>4</v>
       </c>
       <c r="E82">
         <v>2.2200000000000001E-2</v>
@@ -2338,10 +2436,13 @@
         <v>68</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>172</v>
+        <v>184</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
       </c>
       <c r="E83">
         <v>8.8000000000000005E-3</v>
@@ -2356,10 +2457,13 @@
         <v>69</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>174</v>
+        <v>185</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
       </c>
       <c r="E84">
         <v>0.19719999999999999</v>
@@ -2374,10 +2478,13 @@
         <v>70</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>176</v>
+        <v>186</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
       </c>
       <c r="E85">
         <v>7.3000000000000001E-3</v>
@@ -2392,10 +2499,13 @@
         <v>71</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
       </c>
       <c r="E86">
         <v>3.2300000000000002E-2</v>
@@ -2410,10 +2520,13 @@
         <v>72</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>180</v>
+        <v>188</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
       </c>
       <c r="E87">
         <v>1.2E-2</v>
@@ -2428,10 +2541,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>182</v>
+        <v>189</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
       </c>
       <c r="E88">
         <v>8.3999999999999995E-3</v>
@@ -2446,10 +2562,13 @@
         <v>74</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>182</v>
+        <v>189</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
       </c>
       <c r="E89">
         <v>1.6400000000000001E-2</v>
@@ -2464,10 +2583,13 @@
         <v>75</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
       </c>
       <c r="E90">
         <v>1.7000000000000001E-2</v>
@@ -2482,10 +2604,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
       </c>
       <c r="E91">
         <v>4.5999999999999999E-3</v>
@@ -2500,10 +2625,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>189</v>
+        <v>161</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
       </c>
       <c r="E92">
         <v>1.5699999999999999E-2</v>
@@ -2518,10 +2646,13 @@
         <v>78</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>191</v>
+        <v>164</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
       </c>
       <c r="E93">
         <v>3.39E-2</v>

</xml_diff>